<commit_message>
new results && correct rng
heston lines of code (loc) + full comparison
</commit_message>
<xml_diff>
--- a/results/2013.09.02_date_2011_sl_comparison/review.xlsx
+++ b/results/2013.09.02_date_2011_sl_comparison/review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="4890" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Path_cnt</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>40 nm</t>
-  </si>
-  <si>
-    <t>66 nm</t>
   </si>
   <si>
     <t>Core 2 Duo + ML502</t>
@@ -173,7 +170,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -189,9 +186,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,7 +226,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -301,7 +298,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -478,10 +475,10 @@
   <dimension ref="A2:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -601,7 +598,7 @@
         <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -635,7 +632,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4">
         <f>B6/E12</f>
@@ -657,7 +654,7 @@
         <v>1E-8</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I12" t="s">
         <v>12</v>

</xml_diff>